<commit_message>
Added adc section Added frequency checking Modified usart usage to work with stdio.h
</commit_message>
<xml_diff>
--- a/initmaker/documentation/ATSAMD5XE5X pins.xlsx
+++ b/initmaker/documentation/ATSAMD5XE5X pins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="195" windowWidth="9225" windowHeight="2910"/>
+    <workbookView xWindow="120" yWindow="195" windowWidth="9225" windowHeight="2910" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Datasheet" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="100" sheetId="4" r:id="rId4"/>
     <sheet name="120" sheetId="5" r:id="rId5"/>
     <sheet name="128" sheetId="6" r:id="rId6"/>
+    <sheet name="SERCOM" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="test" localSheetId="3">'100'!$A$5:$U$81</definedName>
@@ -224,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4676" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4777" uniqueCount="700">
   <si>
     <t>4</t>
   </si>
@@ -2186,6 +2187,144 @@
   </si>
   <si>
     <t>XOSC1 XOUT Crystal</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>PAD[0]</t>
+  </si>
+  <si>
+    <t>PAD[1]</t>
+  </si>
+  <si>
+    <t>PAD[2]</t>
+  </si>
+  <si>
+    <t>SDA_OUT</t>
+  </si>
+  <si>
+    <t>PAD[3]</t>
+  </si>
+  <si>
+    <t>SCL_OUT</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>SCLK</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>Channels</t>
+  </si>
+  <si>
+    <t>Waveform Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Counter Size</t>
+  </si>
+  <si>
+    <t>Fault</t>
+  </si>
+  <si>
+    <t>Dither</t>
+  </si>
+  <si>
+    <t>Deadtime Insertion</t>
+  </si>
+  <si>
+    <t>Swap</t>
+  </si>
+  <si>
+    <t>Pattern Generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24-bit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16-bit </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TCC Capabilities</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>TXD</t>
+  </si>
+  <si>
+    <t>XCK</t>
+  </si>
+  <si>
+    <t>RXD</t>
+  </si>
+  <si>
+    <t>DIPO:3 DOPO:0</t>
+  </si>
+  <si>
+    <t>DIPO:0 DOPO:2</t>
+  </si>
+  <si>
+    <t>TXPO:0 RXPO:2</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>TXPO:0 RXPO:3</t>
+  </si>
+  <si>
+    <t>RTS</t>
+  </si>
+  <si>
+    <t>CTS</t>
+  </si>
+  <si>
+    <t>TXPO:2 RXPO:1</t>
+  </si>
+  <si>
+    <t>TXPO:3 RXPO:3</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>TXPO:2 RXPO:2</t>
+  </si>
+  <si>
+    <t>TXPO:2 RXPO:3</t>
+  </si>
+  <si>
+    <t>SERCOM Pad Allocation</t>
+  </si>
+  <si>
+    <t>Note: SDA_OUT/SCL_OUT are only needed if you want to bypass the I2C driver</t>
+  </si>
+  <si>
+    <t>Output Matrix</t>
   </si>
 </sst>
 </file>
@@ -2221,7 +2360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2235,6 +2374,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2563,7 +2729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
@@ -2842,14 +3008,14 @@
       <c r="H4" t="s">
         <v>605</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
       <c r="O4" t="s">
         <v>613</v>
       </c>
@@ -6710,7 +6876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView topLeftCell="J29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="V34" sqref="V34:V35"/>
     </sheetView>
   </sheetViews>
@@ -6788,14 +6954,14 @@
       <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
       <c r="J2" t="s">
         <v>613</v>
       </c>
@@ -8105,14 +8271,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="W43" sqref="W43:W44"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
     <col min="12" max="12" width="21.85546875" customWidth="1"/>
     <col min="13" max="13" width="17.85546875" customWidth="1"/>
@@ -8120,10 +8291,13 @@
     <col min="15" max="15" width="19.7109375" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
     <col min="17" max="17" width="24.85546875" customWidth="1"/>
+    <col min="21" max="21" width="22.42578125" customWidth="1"/>
     <col min="23" max="23" width="28.85546875" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>604</v>
       </c>
@@ -8182,7 +8356,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>64</v>
       </c>
@@ -8195,14 +8369,14 @@
       <c r="D2" t="s">
         <v>605</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" t="s">
         <v>613</v>
       </c>
@@ -8243,7 +8417,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -8265,8 +8439,10 @@
       <c r="W3" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="6"/>
+      <c r="Z3" s="5"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -8288,8 +8464,10 @@
       <c r="W4" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="1"/>
+      <c r="Z4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -8308,8 +8486,10 @@
       <c r="I5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" s="1"/>
+      <c r="Z5" s="1"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -8331,8 +8511,10 @@
       <c r="J6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" s="1"/>
+      <c r="Z6" s="1"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -8351,8 +8533,11 @@
       <c r="J7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AB7" s="11"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -8371,8 +8556,11 @@
       <c r="J8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AB8" s="11"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -8394,8 +8582,10 @@
       <c r="V9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9" s="1"/>
+      <c r="Z9" s="1"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -8417,8 +8607,11 @@
       <c r="V10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AB10" s="11"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -8449,8 +8642,11 @@
       <c r="V11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AB11" s="11"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -8481,8 +8677,11 @@
       <c r="V12" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AB12" s="7"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -8516,8 +8715,11 @@
       <c r="V13" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AB13" s="7"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
@@ -8548,8 +8750,10 @@
       <c r="V14" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X14" s="1"/>
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -8586,8 +8790,10 @@
       <c r="V15" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -8621,8 +8827,11 @@
       <c r="V16" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AB16" s="11"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -8671,8 +8880,11 @@
       <c r="V17" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AB17" s="11"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>65</v>
       </c>
@@ -8721,8 +8933,11 @@
       <c r="V18" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AB18" s="7"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>74</v>
       </c>
@@ -8771,8 +8986,11 @@
       <c r="V19" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AB19" s="7"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>85</v>
       </c>
@@ -8821,8 +9039,10 @@
       <c r="V20" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X20" s="1"/>
+      <c r="Z20" s="1"/>
+    </row>
+    <row r="21" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>117</v>
       </c>
@@ -8862,8 +9082,10 @@
       <c r="V21" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X21" s="1"/>
+      <c r="Z21" s="1"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>129</v>
       </c>
@@ -8903,8 +9125,10 @@
       <c r="V22" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X22" s="1"/>
+      <c r="Z22" s="1"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>238</v>
       </c>
@@ -8944,8 +9168,10 @@
       <c r="U23" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X23" s="1"/>
+      <c r="Z23" s="1"/>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>156</v>
       </c>
@@ -8985,8 +9211,10 @@
       <c r="U24" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X24" s="1"/>
+      <c r="Z24" s="1"/>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>139</v>
       </c>
@@ -9029,8 +9257,10 @@
       <c r="V25" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X25" s="1"/>
+      <c r="Z25" s="1"/>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>144</v>
       </c>
@@ -9073,8 +9303,10 @@
       <c r="V26" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X26" s="1"/>
+      <c r="Z26" s="1"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>148</v>
       </c>
@@ -9114,8 +9346,10 @@
       <c r="U27" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X27" s="1"/>
+      <c r="Z27" s="1"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>152</v>
       </c>
@@ -9155,8 +9389,10 @@
       <c r="U28" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X28" s="1"/>
+      <c r="Z28" s="1"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>343</v>
       </c>
@@ -9196,8 +9432,10 @@
       <c r="W29" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X29" s="1"/>
+      <c r="Z29" s="1"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>215</v>
       </c>
@@ -9234,8 +9472,11 @@
       <c r="W30" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AB30" s="11"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>186</v>
       </c>
@@ -9278,8 +9519,11 @@
       <c r="V31" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AB31" s="11"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>201</v>
       </c>
@@ -9322,8 +9566,10 @@
       <c r="V32" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X32" s="1"/>
+      <c r="Z32" s="1"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>271</v>
       </c>
@@ -9366,8 +9612,10 @@
       <c r="V33" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X33" s="1"/>
+      <c r="Z33" s="1"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>385</v>
       </c>
@@ -9410,8 +9658,10 @@
       <c r="V34" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X34" s="1"/>
+      <c r="Z34" s="1"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>217</v>
       </c>
@@ -9448,8 +9698,10 @@
       <c r="V35" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X35" s="1"/>
+      <c r="Z35" s="1"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>229</v>
       </c>
@@ -9486,8 +9738,10 @@
       <c r="V36" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X36" s="1"/>
+      <c r="Z36" s="1"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>241</v>
       </c>
@@ -9530,8 +9784,10 @@
       <c r="T37" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X37" s="1"/>
+      <c r="Z37" s="1"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>251</v>
       </c>
@@ -9574,8 +9830,10 @@
       <c r="T38" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X38" s="1"/>
+      <c r="Z38" s="1"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>261</v>
       </c>
@@ -9618,8 +9876,10 @@
       <c r="V39" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X39" s="1"/>
+      <c r="Z39" s="1"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>273</v>
       </c>
@@ -9665,8 +9925,10 @@
       <c r="V40" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X40" s="1"/>
+      <c r="Z40" s="1"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>320</v>
       </c>
@@ -9703,8 +9965,10 @@
       <c r="V41" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X41" s="1"/>
+      <c r="Z41" s="1"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>326</v>
       </c>
@@ -9738,8 +10002,10 @@
       <c r="V42" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X42" s="1"/>
+      <c r="Z42" s="1"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>291</v>
       </c>
@@ -9776,8 +10042,10 @@
       <c r="W43" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X43" s="1"/>
+      <c r="Z43" s="1"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>295</v>
       </c>
@@ -9811,8 +10079,10 @@
       <c r="W44" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X44" s="1"/>
+      <c r="Z44" s="1"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>299</v>
       </c>
@@ -9831,8 +10101,10 @@
       <c r="U45" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X45" s="1"/>
+      <c r="Z45" s="1"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>312</v>
       </c>
@@ -9869,8 +10141,10 @@
       <c r="V46" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X46" s="1"/>
+      <c r="Z46" s="1"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>316</v>
       </c>
@@ -9901,8 +10175,10 @@
       <c r="V47" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X47" s="1"/>
+      <c r="Z47" s="1"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>322</v>
       </c>
@@ -9933,8 +10209,10 @@
       <c r="P48" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X48" s="1"/>
+      <c r="Z48" s="1"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>328</v>
       </c>
@@ -9962,8 +10240,10 @@
       <c r="O49" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X49" s="1"/>
+      <c r="Z49" s="1"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>336</v>
       </c>
@@ -9991,8 +10271,10 @@
       <c r="V50" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X50" s="1"/>
+      <c r="Z50" s="1"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>345</v>
       </c>
@@ -10020,8 +10302,10 @@
       <c r="V51" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X51" s="1"/>
+      <c r="Z51" s="1"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>352</v>
       </c>
@@ -10052,8 +10336,10 @@
       <c r="V52" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="X52" s="1"/>
+      <c r="Z52" s="1"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>64</v>
       </c>
@@ -10082,6 +10368,8 @@
       <c r="M53" t="s">
         <v>441</v>
       </c>
+      <c r="X53" s="6"/>
+      <c r="Z53" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10174,14 +10462,14 @@
       <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
       <c r="J2" t="s">
         <v>613</v>
       </c>
@@ -12627,14 +12915,14 @@
       <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
       <c r="J2" t="s">
         <v>613</v>
       </c>
@@ -15427,14 +15715,14 @@
       <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
       <c r="J2" t="s">
         <v>613</v>
       </c>
@@ -18141,4 +18429,441 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>697</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>614</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>688</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>685</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>687</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>689</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>695</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>696</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>654</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>664</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>665</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>655</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>666</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>659</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>690</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>662</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>691</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="14" t="s">
+        <v>698</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>680</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>618</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>669</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>671</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>672</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>699</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>674</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>676</v>
+      </c>
+      <c r="E18" t="s">
+        <v>677</v>
+      </c>
+      <c r="F18" t="s">
+        <v>677</v>
+      </c>
+      <c r="G18" t="s">
+        <v>677</v>
+      </c>
+      <c r="H18" t="s">
+        <v>677</v>
+      </c>
+      <c r="I18" t="s">
+        <v>677</v>
+      </c>
+      <c r="J18" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>676</v>
+      </c>
+      <c r="E19" t="s">
+        <v>677</v>
+      </c>
+      <c r="F19" t="s">
+        <v>677</v>
+      </c>
+      <c r="G19" t="s">
+        <v>677</v>
+      </c>
+      <c r="H19" t="s">
+        <v>677</v>
+      </c>
+      <c r="I19" t="s">
+        <v>677</v>
+      </c>
+      <c r="J19" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>678</v>
+      </c>
+      <c r="E20" t="s">
+        <v>677</v>
+      </c>
+      <c r="F20" t="s">
+        <v>679</v>
+      </c>
+      <c r="G20" t="s">
+        <v>677</v>
+      </c>
+      <c r="H20" t="s">
+        <v>679</v>
+      </c>
+      <c r="I20" t="s">
+        <v>679</v>
+      </c>
+      <c r="J20" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>678</v>
+      </c>
+      <c r="E21" t="s">
+        <v>677</v>
+      </c>
+      <c r="F21" t="s">
+        <v>679</v>
+      </c>
+      <c r="G21" t="s">
+        <v>679</v>
+      </c>
+      <c r="H21" t="s">
+        <v>679</v>
+      </c>
+      <c r="I21" t="s">
+        <v>679</v>
+      </c>
+      <c r="J21" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>678</v>
+      </c>
+      <c r="E22" t="s">
+        <v>677</v>
+      </c>
+      <c r="F22" t="s">
+        <v>679</v>
+      </c>
+      <c r="G22" t="s">
+        <v>679</v>
+      </c>
+      <c r="H22" t="s">
+        <v>679</v>
+      </c>
+      <c r="I22" t="s">
+        <v>679</v>
+      </c>
+      <c r="J22" t="s">
+        <v>679</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B9:D11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to Version 2.0.0 see documentation/Changes 2.0.txt
</commit_message>
<xml_diff>
--- a/initmaker/documentation/ATSAMD5XE5X pins.xlsx
+++ b/initmaker/documentation/ATSAMD5XE5X pins.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="195" windowWidth="9225" windowHeight="2910" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="198" windowWidth="9228" windowHeight="2910" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Datasheet" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="test" localSheetId="2">'64'!$A$5:$V$52</definedName>
     <definedName name="test" localSheetId="0">Datasheet!$A$8:$Z$102</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4777" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4790" uniqueCount="704">
   <si>
     <t>4</t>
   </si>
@@ -2318,13 +2318,25 @@
     <t>TXPO:2 RXPO:3</t>
   </si>
   <si>
-    <t>SERCOM Pad Allocation</t>
-  </si>
-  <si>
     <t>Note: SDA_OUT/SCL_OUT are only needed if you want to bypass the I2C driver</t>
   </si>
   <si>
     <t>Output Matrix</t>
+  </si>
+  <si>
+    <t>DIPO:0 DOPO:1</t>
+  </si>
+  <si>
+    <t>DIPO:2 DOPO:3</t>
+  </si>
+  <si>
+    <t>SAMD SERCOM Pad Allocation</t>
+  </si>
+  <si>
+    <t>SPI*</t>
+  </si>
+  <si>
+    <t>Note SPI* not valid for SAMD51</t>
   </si>
 </sst>
 </file>
@@ -2360,7 +2372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2392,6 +2404,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2733,35 +2748,35 @@
       <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.41796875" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.26171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.68359375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.41796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.41796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.15625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="16.578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.83984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.15625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="28" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="44.140625" customWidth="1"/>
+    <col min="22" max="22" width="10.83984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.83984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="44.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>636</v>
       </c>
@@ -2841,7 +2856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2924,7 +2939,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
         <v>604</v>
       </c>
@@ -2983,7 +2998,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>48</v>
       </c>
@@ -3008,14 +3023,14 @@
       <c r="H4" t="s">
         <v>605</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="13" t="s">
         <v>612</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
       <c r="O4" t="s">
         <v>613</v>
       </c>
@@ -3053,7 +3068,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -3088,7 +3103,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -3123,7 +3138,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3146,7 +3161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3169,7 +3184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -3192,7 +3207,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -3224,7 +3239,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -3259,7 +3274,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -3289,7 +3304,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>11</v>
@@ -3319,7 +3334,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -3340,7 +3355,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -3361,7 +3376,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -3394,7 +3409,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>26</v>
@@ -3427,7 +3442,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -3471,7 +3486,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -3515,7 +3530,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -3562,7 +3577,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -3606,7 +3621,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -3656,7 +3671,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -3703,7 +3718,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3727,7 +3742,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3750,7 +3765,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3776,7 +3791,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3802,7 +3817,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
@@ -3864,7 +3879,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -3926,7 +3941,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -3988,7 +4003,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>51</v>
       </c>
@@ -4050,7 +4065,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
@@ -4103,7 +4118,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>85</v>
       </c>
@@ -4156,7 +4171,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>238</v>
@@ -4207,7 +4222,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
         <v>156</v>
@@ -4258,7 +4273,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>139</v>
@@ -4312,7 +4327,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>144</v>
@@ -4366,7 +4381,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -4393,7 +4408,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -4420,7 +4435,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -4447,7 +4462,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -4474,7 +4489,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -4495,7 +4510,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -4527,7 +4542,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -4562,7 +4577,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -4600,7 +4615,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -4635,7 +4650,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -4673,7 +4688,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -4764,7 +4779,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>107</v>
       </c>
@@ -4817,7 +4832,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>117</v>
       </c>
@@ -4870,7 +4885,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>129</v>
       </c>
@@ -4920,7 +4935,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>238</v>
       </c>
@@ -4976,7 +4991,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>156</v>
       </c>
@@ -5032,7 +5047,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>139</v>
       </c>
@@ -5088,7 +5103,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>144</v>
       </c>
@@ -5144,7 +5159,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -5179,7 +5194,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -5214,7 +5229,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -5249,7 +5264,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -5281,7 +5296,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -5313,7 +5328,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -5345,7 +5360,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -5375,7 +5390,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -5405,7 +5420,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -5435,7 +5450,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -5465,7 +5480,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
         <v>217</v>
@@ -5513,7 +5528,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
         <v>229</v>
@@ -5561,7 +5576,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -5599,7 +5614,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -5637,7 +5652,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -5675,7 +5690,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -5710,7 +5725,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>148</v>
       </c>
@@ -5766,7 +5781,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>152</v>
       </c>
@@ -5822,7 +5837,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>343</v>
       </c>
@@ -5878,7 +5893,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>215</v>
       </c>
@@ -5937,7 +5952,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>158</v>
       </c>
@@ -5987,7 +6002,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>172</v>
       </c>
@@ -6034,7 +6049,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>271</v>
       </c>
@@ -6084,7 +6099,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>385</v>
       </c>
@@ -6131,7 +6146,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -6163,7 +6178,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -6195,7 +6210,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -6222,7 +6237,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -6249,7 +6264,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -6279,7 +6294,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -6309,7 +6324,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -6338,7 +6353,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -6367,7 +6382,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -6390,7 +6405,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -6422,7 +6437,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -6451,7 +6466,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
         <v>217</v>
       </c>
@@ -6483,7 +6498,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
         <v>320</v>
       </c>
@@ -6533,7 +6548,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
         <v>326</v>
       </c>
@@ -6577,7 +6592,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1"/>
       <c r="B96" s="1" t="s">
         <v>322</v>
@@ -6619,7 +6634,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1"/>
       <c r="B97" s="1" t="s">
         <v>328</v>
@@ -6658,7 +6673,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -6679,7 +6694,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -6700,7 +6715,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1"/>
       <c r="B100" s="1" t="s">
         <v>336</v>
@@ -6739,7 +6754,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1"/>
       <c r="B101" s="1" t="s">
         <v>345</v>
@@ -6778,7 +6793,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1" t="s">
         <v>283</v>
       </c>
@@ -6822,7 +6837,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="3">
         <v>48</v>
       </c>
@@ -6880,12 +6895,12 @@
       <selection activeCell="V34" sqref="V34:V35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="22" max="22" width="29.5703125" customWidth="1"/>
+    <col min="22" max="22" width="29.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>604</v>
       </c>
@@ -6944,7 +6959,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>48</v>
       </c>
@@ -6954,14 +6969,14 @@
       <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>612</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
       <c r="J2" t="s">
         <v>613</v>
       </c>
@@ -7002,7 +7017,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -7010,7 +7025,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -7030,7 +7045,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -7050,7 +7065,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -7067,7 +7082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -7087,7 +7102,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -7116,7 +7131,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -7145,7 +7160,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -7177,7 +7192,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -7206,7 +7221,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -7241,7 +7256,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -7273,7 +7288,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -7320,7 +7335,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
@@ -7367,7 +7382,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -7414,7 +7429,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
@@ -7461,7 +7476,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
@@ -7499,7 +7514,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>85</v>
       </c>
@@ -7537,7 +7552,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
@@ -7575,7 +7590,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>107</v>
       </c>
@@ -7613,7 +7628,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
@@ -7651,7 +7666,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>129</v>
       </c>
@@ -7686,7 +7701,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>238</v>
       </c>
@@ -7727,7 +7742,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>156</v>
       </c>
@@ -7768,7 +7783,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>139</v>
       </c>
@@ -7809,7 +7824,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>144</v>
       </c>
@@ -7850,7 +7865,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>148</v>
       </c>
@@ -7891,7 +7906,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>152</v>
       </c>
@@ -7932,7 +7947,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>343</v>
       </c>
@@ -7973,7 +7988,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>215</v>
       </c>
@@ -8017,7 +8032,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>158</v>
       </c>
@@ -8052,7 +8067,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>172</v>
       </c>
@@ -8084,7 +8099,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>271</v>
       </c>
@@ -8119,7 +8134,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>385</v>
       </c>
@@ -8151,7 +8166,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>217</v>
       </c>
@@ -8168,7 +8183,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>320</v>
       </c>
@@ -8203,7 +8218,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>326</v>
       </c>
@@ -8232,7 +8247,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
         <v>283</v>
       </c>
@@ -8273,31 +8288,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.578125" customWidth="1"/>
+    <col min="5" max="5" width="18.26171875" customWidth="1"/>
+    <col min="6" max="6" width="14.26171875" customWidth="1"/>
+    <col min="7" max="7" width="14.15625" customWidth="1"/>
+    <col min="8" max="8" width="13.68359375" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="21.83984375" customWidth="1"/>
+    <col min="13" max="13" width="17.83984375" customWidth="1"/>
+    <col min="14" max="14" width="13.83984375" customWidth="1"/>
+    <col min="15" max="15" width="19.68359375" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" customWidth="1"/>
-    <col min="23" max="23" width="28.85546875" customWidth="1"/>
-    <col min="24" max="24" width="10.85546875" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" customWidth="1"/>
+    <col min="17" max="17" width="24.83984375" customWidth="1"/>
+    <col min="21" max="21" width="22.41796875" customWidth="1"/>
+    <col min="23" max="23" width="28.83984375" customWidth="1"/>
+    <col min="24" max="24" width="10.83984375" customWidth="1"/>
+    <col min="25" max="25" width="17.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>604</v>
       </c>
@@ -8356,7 +8371,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>64</v>
       </c>
@@ -8369,14 +8384,14 @@
       <c r="D2" t="s">
         <v>605</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>612</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
       <c r="K2" t="s">
         <v>613</v>
       </c>
@@ -8417,7 +8432,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -8442,7 +8457,7 @@
       <c r="X3" s="6"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -8467,7 +8482,7 @@
       <c r="X4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -8489,7 +8504,7 @@
       <c r="X5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -8514,7 +8529,7 @@
       <c r="X6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -8537,7 +8552,7 @@
       <c r="Z7" s="1"/>
       <c r="AB7" s="11"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -8560,7 +8575,7 @@
       <c r="Z8" s="1"/>
       <c r="AB8" s="11"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -8585,7 +8600,7 @@
       <c r="X9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -8611,7 +8626,7 @@
       <c r="Z10" s="1"/>
       <c r="AB10" s="11"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -8646,7 +8661,7 @@
       <c r="Z11" s="1"/>
       <c r="AB11" s="11"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -8681,7 +8696,7 @@
       <c r="Z12" s="1"/>
       <c r="AB12" s="7"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
@@ -8719,7 +8734,7 @@
       <c r="Z13" s="1"/>
       <c r="AB13" s="7"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>63</v>
       </c>
@@ -8753,7 +8768,7 @@
       <c r="X14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -8793,7 +8808,7 @@
       <c r="X15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -8831,7 +8846,7 @@
       <c r="Z16" s="1"/>
       <c r="AB16" s="11"/>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
@@ -8884,7 +8899,7 @@
       <c r="Z17" s="1"/>
       <c r="AB17" s="11"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>65</v>
       </c>
@@ -8937,7 +8952,7 @@
       <c r="Z18" s="1"/>
       <c r="AB18" s="7"/>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>74</v>
       </c>
@@ -8990,7 +9005,7 @@
       <c r="Z19" s="1"/>
       <c r="AB19" s="7"/>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>85</v>
       </c>
@@ -9042,7 +9057,7 @@
       <c r="X20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>117</v>
       </c>
@@ -9085,7 +9100,7 @@
       <c r="X21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>129</v>
       </c>
@@ -9128,7 +9143,7 @@
       <c r="X22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>238</v>
       </c>
@@ -9171,7 +9186,7 @@
       <c r="X23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>156</v>
       </c>
@@ -9214,7 +9229,7 @@
       <c r="X24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>139</v>
       </c>
@@ -9260,7 +9275,7 @@
       <c r="X25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
         <v>144</v>
       </c>
@@ -9306,7 +9321,7 @@
       <c r="X26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>148</v>
       </c>
@@ -9349,7 +9364,7 @@
       <c r="X27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>152</v>
       </c>
@@ -9392,7 +9407,7 @@
       <c r="X28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>343</v>
       </c>
@@ -9435,7 +9450,7 @@
       <c r="X29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>215</v>
       </c>
@@ -9476,7 +9491,7 @@
       <c r="Z30" s="1"/>
       <c r="AB30" s="11"/>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>186</v>
       </c>
@@ -9523,7 +9538,7 @@
       <c r="Z31" s="1"/>
       <c r="AB31" s="11"/>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>201</v>
       </c>
@@ -9569,7 +9584,7 @@
       <c r="X32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>271</v>
       </c>
@@ -9615,7 +9630,7 @@
       <c r="X33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>385</v>
       </c>
@@ -9661,7 +9676,7 @@
       <c r="X34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
         <v>217</v>
       </c>
@@ -9701,7 +9716,7 @@
       <c r="X35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>229</v>
       </c>
@@ -9741,7 +9756,7 @@
       <c r="X36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>241</v>
       </c>
@@ -9787,7 +9802,7 @@
       <c r="X37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>251</v>
       </c>
@@ -9833,7 +9848,7 @@
       <c r="X38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
         <v>261</v>
       </c>
@@ -9879,7 +9894,7 @@
       <c r="X39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
         <v>273</v>
       </c>
@@ -9928,7 +9943,7 @@
       <c r="X40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
         <v>320</v>
       </c>
@@ -9968,7 +9983,7 @@
       <c r="X41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
         <v>326</v>
       </c>
@@ -10005,7 +10020,7 @@
       <c r="X42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
         <v>291</v>
       </c>
@@ -10045,7 +10060,7 @@
       <c r="X43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
         <v>295</v>
       </c>
@@ -10082,7 +10097,7 @@
       <c r="X44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
         <v>299</v>
       </c>
@@ -10104,7 +10119,7 @@
       <c r="X45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
         <v>312</v>
       </c>
@@ -10144,7 +10159,7 @@
       <c r="X46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
         <v>316</v>
       </c>
@@ -10178,7 +10193,7 @@
       <c r="X47" s="1"/>
       <c r="Z47" s="1"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
         <v>322</v>
       </c>
@@ -10212,7 +10227,7 @@
       <c r="X48" s="1"/>
       <c r="Z48" s="1"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
         <v>328</v>
       </c>
@@ -10243,7 +10258,7 @@
       <c r="X49" s="1"/>
       <c r="Z49" s="1"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
         <v>336</v>
       </c>
@@ -10274,7 +10289,7 @@
       <c r="X50" s="1"/>
       <c r="Z50" s="1"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
         <v>345</v>
       </c>
@@ -10305,7 +10320,7 @@
       <c r="X51" s="1"/>
       <c r="Z51" s="1"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
         <v>352</v>
       </c>
@@ -10339,7 +10354,7 @@
       <c r="X52" s="1"/>
       <c r="Z52" s="1"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3">
         <v>64</v>
       </c>
@@ -10388,12 +10403,12 @@
       <selection activeCell="V65" sqref="V65:V66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="22" max="22" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>604</v>
       </c>
@@ -10452,7 +10467,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -10462,14 +10477,14 @@
       <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>612</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
       <c r="J2" t="s">
         <v>613</v>
       </c>
@@ -10510,7 +10525,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -10530,7 +10545,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -10550,7 +10565,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -10564,7 +10579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -10578,7 +10593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -10592,7 +10607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -10609,7 +10624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -10629,7 +10644,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -10646,7 +10661,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -10663,7 +10678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -10683,7 +10698,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>63</v>
       </c>
@@ -10703,7 +10718,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
@@ -10732,7 +10747,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
@@ -10761,7 +10776,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
@@ -10793,7 +10808,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -10822,7 +10837,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>74</v>
       </c>
@@ -10857,7 +10872,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>85</v>
       </c>
@@ -10889,7 +10904,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
@@ -10903,7 +10918,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>107</v>
       </c>
@@ -10920,7 +10935,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>117</v>
       </c>
@@ -10937,7 +10952,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>156</v>
       </c>
@@ -10984,7 +10999,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>139</v>
       </c>
@@ -11031,7 +11046,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>144</v>
       </c>
@@ -11078,7 +11093,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>148</v>
       </c>
@@ -11125,7 +11140,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>215</v>
       </c>
@@ -11163,7 +11178,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>158</v>
       </c>
@@ -11201,7 +11216,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>172</v>
       </c>
@@ -11239,7 +11254,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>186</v>
       </c>
@@ -11277,7 +11292,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>201</v>
       </c>
@@ -11318,7 +11333,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>271</v>
       </c>
@@ -11359,7 +11374,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>229</v>
       </c>
@@ -11382,7 +11397,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>241</v>
       </c>
@@ -11408,7 +11423,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>251</v>
       </c>
@@ -11437,7 +11452,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>261</v>
       </c>
@@ -11463,7 +11478,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>273</v>
       </c>
@@ -11492,7 +11507,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>320</v>
       </c>
@@ -11521,7 +11536,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>326</v>
       </c>
@@ -11559,7 +11574,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>283</v>
       </c>
@@ -11597,7 +11612,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>287</v>
       </c>
@@ -11635,7 +11650,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>291</v>
       </c>
@@ -11670,7 +11685,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>302</v>
       </c>
@@ -11711,7 +11726,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>366</v>
       </c>
@@ -11752,7 +11767,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>376</v>
       </c>
@@ -11793,7 +11808,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>305</v>
       </c>
@@ -11834,7 +11849,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>308</v>
       </c>
@@ -11860,7 +11875,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>312</v>
       </c>
@@ -11886,7 +11901,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>316</v>
       </c>
@@ -11912,7 +11927,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>322</v>
       </c>
@@ -11935,7 +11950,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>328</v>
       </c>
@@ -11958,7 +11973,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>336</v>
       </c>
@@ -11981,7 +11996,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>436</v>
       </c>
@@ -12016,7 +12031,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>442</v>
       </c>
@@ -12051,7 +12066,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>358</v>
       </c>
@@ -12080,7 +12095,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>368</v>
       </c>
@@ -12109,7 +12124,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>378</v>
       </c>
@@ -12138,7 +12153,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>387</v>
       </c>
@@ -12164,7 +12179,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>395</v>
       </c>
@@ -12205,7 +12220,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>400</v>
       </c>
@@ -12246,7 +12261,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>405</v>
       </c>
@@ -12287,7 +12302,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>410</v>
       </c>
@@ -12331,7 +12346,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>414</v>
       </c>
@@ -12366,7 +12381,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>419</v>
       </c>
@@ -12398,7 +12413,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>508</v>
       </c>
@@ -12433,7 +12448,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
         <v>513</v>
       </c>
@@ -12465,7 +12480,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
         <v>430</v>
       </c>
@@ -12488,7 +12503,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>433</v>
       </c>
@@ -12511,7 +12526,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
         <v>438</v>
       </c>
@@ -12531,7 +12546,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
         <v>444</v>
       </c>
@@ -12551,7 +12566,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>450</v>
       </c>
@@ -12565,7 +12580,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>455</v>
       </c>
@@ -12588,7 +12603,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>459</v>
       </c>
@@ -12608,7 +12623,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>463</v>
       </c>
@@ -12625,7 +12640,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>490</v>
       </c>
@@ -12660,7 +12675,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>498</v>
       </c>
@@ -12689,7 +12704,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>504</v>
       </c>
@@ -12718,7 +12733,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>576</v>
       </c>
@@ -12744,7 +12759,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>589</v>
       </c>
@@ -12770,7 +12785,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>510</v>
       </c>
@@ -12796,7 +12811,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>514</v>
       </c>
@@ -12841,12 +12856,12 @@
       <selection activeCell="A77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="22" max="22" width="33.7109375" customWidth="1"/>
+    <col min="22" max="22" width="33.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>604</v>
       </c>
@@ -12905,7 +12920,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>120</v>
       </c>
@@ -12915,14 +12930,14 @@
       <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>612</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
       <c r="J2" t="s">
         <v>613</v>
       </c>
@@ -12963,7 +12978,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>502</v>
       </c>
@@ -12983,7 +12998,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>496</v>
       </c>
@@ -13003,7 +13018,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -13017,7 +13032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -13031,7 +13046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -13045,7 +13060,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -13062,7 +13077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -13082,7 +13097,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -13099,7 +13114,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -13116,7 +13131,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -13130,7 +13145,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -13144,7 +13159,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -13164,7 +13179,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>64</v>
       </c>
@@ -13184,7 +13199,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>73</v>
       </c>
@@ -13213,7 +13228,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>84</v>
       </c>
@@ -13242,7 +13257,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>95</v>
       </c>
@@ -13274,7 +13289,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>106</v>
       </c>
@@ -13303,7 +13318,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>116</v>
       </c>
@@ -13338,7 +13353,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>128</v>
       </c>
@@ -13370,7 +13385,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>138</v>
       </c>
@@ -13387,7 +13402,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>143</v>
       </c>
@@ -13401,7 +13416,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>147</v>
       </c>
@@ -13418,7 +13433,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>151</v>
       </c>
@@ -13435,7 +13450,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>157</v>
       </c>
@@ -13482,7 +13497,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>171</v>
       </c>
@@ -13529,7 +13544,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>185</v>
       </c>
@@ -13576,7 +13591,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>200</v>
       </c>
@@ -13623,7 +13638,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>216</v>
       </c>
@@ -13661,7 +13676,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>228</v>
       </c>
@@ -13699,7 +13714,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>240</v>
       </c>
@@ -13737,7 +13752,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>250</v>
       </c>
@@ -13775,7 +13790,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>260</v>
       </c>
@@ -13816,7 +13831,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>272</v>
       </c>
@@ -13857,7 +13872,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>282</v>
       </c>
@@ -13877,7 +13892,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>286</v>
       </c>
@@ -13897,7 +13912,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>290</v>
       </c>
@@ -13917,7 +13932,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>294</v>
       </c>
@@ -13937,7 +13952,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>298</v>
       </c>
@@ -13951,7 +13966,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>301</v>
       </c>
@@ -13974,7 +13989,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>304</v>
       </c>
@@ -14000,7 +14015,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>307</v>
       </c>
@@ -14029,7 +14044,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>311</v>
       </c>
@@ -14055,7 +14070,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>315</v>
       </c>
@@ -14084,7 +14099,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>321</v>
       </c>
@@ -14113,7 +14128,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>327</v>
       </c>
@@ -14151,7 +14166,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>335</v>
       </c>
@@ -14189,7 +14204,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>344</v>
       </c>
@@ -14227,7 +14242,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>351</v>
       </c>
@@ -14262,7 +14277,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>357</v>
       </c>
@@ -14303,7 +14318,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>367</v>
       </c>
@@ -14344,7 +14359,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>377</v>
       </c>
@@ -14385,7 +14400,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>386</v>
       </c>
@@ -14426,7 +14441,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>394</v>
       </c>
@@ -14452,7 +14467,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>399</v>
       </c>
@@ -14478,7 +14493,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>404</v>
       </c>
@@ -14504,7 +14519,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>409</v>
       </c>
@@ -14527,7 +14542,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>413</v>
       </c>
@@ -14550,7 +14565,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>418</v>
       </c>
@@ -14573,7 +14588,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>423</v>
       </c>
@@ -14596,7 +14611,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>426</v>
       </c>
@@ -14619,7 +14634,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>429</v>
       </c>
@@ -14642,7 +14657,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>432</v>
       </c>
@@ -14665,7 +14680,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>437</v>
       </c>
@@ -14700,7 +14715,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>443</v>
       </c>
@@ -14735,7 +14750,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>449</v>
       </c>
@@ -14764,7 +14779,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>454</v>
       </c>
@@ -14793,7 +14808,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>454</v>
       </c>
@@ -14822,7 +14837,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
         <v>462</v>
       </c>
@@ -14848,7 +14863,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>467</v>
       </c>
@@ -14889,7 +14904,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>475</v>
       </c>
@@ -14930,7 +14945,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>483</v>
       </c>
@@ -14971,7 +14986,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>489</v>
       </c>
@@ -15015,7 +15030,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>497</v>
       </c>
@@ -15050,7 +15065,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>503</v>
       </c>
@@ -15082,7 +15097,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>509</v>
       </c>
@@ -15117,7 +15132,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>489</v>
       </c>
@@ -15149,7 +15164,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>516</v>
       </c>
@@ -15172,7 +15187,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>519</v>
       </c>
@@ -15195,7 +15210,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>522</v>
       </c>
@@ -15215,7 +15230,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
         <v>525</v>
       </c>
@@ -15235,7 +15250,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
         <v>528</v>
       </c>
@@ -15258,7 +15273,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
         <v>531</v>
       </c>
@@ -15281,7 +15296,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
         <v>534</v>
       </c>
@@ -15301,7 +15316,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
         <v>538</v>
       </c>
@@ -15321,7 +15336,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
         <v>542</v>
       </c>
@@ -15335,7 +15350,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
         <v>546</v>
       </c>
@@ -15358,7 +15373,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
         <v>551</v>
       </c>
@@ -15378,7 +15393,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
         <v>556</v>
       </c>
@@ -15395,7 +15410,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
         <v>561</v>
       </c>
@@ -15430,7 +15445,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
         <v>567</v>
       </c>
@@ -15459,7 +15474,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
         <v>572</v>
       </c>
@@ -15488,7 +15503,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
         <v>577</v>
       </c>
@@ -15514,7 +15529,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
         <v>580</v>
       </c>
@@ -15528,7 +15543,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
         <v>584</v>
       </c>
@@ -15542,7 +15557,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1" t="s">
         <v>512</v>
       </c>
@@ -15568,7 +15583,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
         <v>555</v>
       </c>
@@ -15594,7 +15609,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
         <v>507</v>
       </c>
@@ -15639,14 +15654,14 @@
       <selection activeCell="L77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.83984375" customWidth="1"/>
+    <col min="12" max="12" width="12.578125" customWidth="1"/>
     <col min="22" max="22" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>604</v>
       </c>
@@ -15705,7 +15720,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>128</v>
       </c>
@@ -15715,14 +15730,14 @@
       <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>612</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
       <c r="J2" t="s">
         <v>613</v>
       </c>
@@ -15763,7 +15778,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -15783,7 +15798,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -15803,7 +15818,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -15817,7 +15832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -15831,7 +15846,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -15845,7 +15860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -15862,7 +15877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -15882,7 +15897,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -15899,7 +15914,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -15916,7 +15931,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -15930,7 +15945,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -15944,7 +15959,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
@@ -15964,7 +15979,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
@@ -15984,7 +15999,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>74</v>
       </c>
@@ -16013,7 +16028,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
@@ -16042,7 +16057,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>96</v>
       </c>
@@ -16074,7 +16089,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>107</v>
       </c>
@@ -16103,7 +16118,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>117</v>
       </c>
@@ -16138,7 +16153,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>129</v>
       </c>
@@ -16170,7 +16185,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>139</v>
       </c>
@@ -16187,7 +16202,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>144</v>
       </c>
@@ -16201,7 +16216,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>148</v>
       </c>
@@ -16218,7 +16233,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>152</v>
       </c>
@@ -16235,7 +16250,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>158</v>
       </c>
@@ -16282,7 +16297,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>172</v>
       </c>
@@ -16329,7 +16344,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>186</v>
       </c>
@@ -16376,7 +16391,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>201</v>
       </c>
@@ -16423,7 +16438,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>217</v>
       </c>
@@ -16461,7 +16476,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>229</v>
       </c>
@@ -16499,7 +16514,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>241</v>
       </c>
@@ -16537,7 +16552,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>251</v>
       </c>
@@ -16575,7 +16590,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>261</v>
       </c>
@@ -16616,7 +16631,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>273</v>
       </c>
@@ -16657,7 +16672,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>283</v>
       </c>
@@ -16677,7 +16692,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>287</v>
       </c>
@@ -16697,7 +16712,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>291</v>
       </c>
@@ -16717,7 +16732,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>295</v>
       </c>
@@ -16737,7 +16752,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>299</v>
       </c>
@@ -16751,7 +16766,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>302</v>
       </c>
@@ -16774,7 +16789,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>305</v>
       </c>
@@ -16800,7 +16815,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>308</v>
       </c>
@@ -16829,7 +16844,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>312</v>
       </c>
@@ -16855,7 +16870,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>316</v>
       </c>
@@ -16884,7 +16899,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>322</v>
       </c>
@@ -16913,7 +16928,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>328</v>
       </c>
@@ -16951,7 +16966,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>336</v>
       </c>
@@ -16989,7 +17004,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>345</v>
       </c>
@@ -17027,7 +17042,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>352</v>
       </c>
@@ -17062,7 +17077,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>358</v>
       </c>
@@ -17103,7 +17118,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>368</v>
       </c>
@@ -17144,7 +17159,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>378</v>
       </c>
@@ -17185,7 +17200,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>387</v>
       </c>
@@ -17226,7 +17241,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>395</v>
       </c>
@@ -17252,7 +17267,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>400</v>
       </c>
@@ -17278,7 +17293,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>405</v>
       </c>
@@ -17304,7 +17319,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>410</v>
       </c>
@@ -17327,7 +17342,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>414</v>
       </c>
@@ -17350,7 +17365,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>419</v>
       </c>
@@ -17373,7 +17388,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>424</v>
       </c>
@@ -17396,7 +17411,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>427</v>
       </c>
@@ -17419,7 +17434,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>430</v>
       </c>
@@ -17442,7 +17457,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>433</v>
       </c>
@@ -17465,7 +17480,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>438</v>
       </c>
@@ -17500,7 +17515,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>444</v>
       </c>
@@ -17535,7 +17550,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>450</v>
       </c>
@@ -17564,7 +17579,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>455</v>
       </c>
@@ -17593,7 +17608,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>459</v>
       </c>
@@ -17622,7 +17637,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>463</v>
       </c>
@@ -17648,7 +17663,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>468</v>
       </c>
@@ -17689,7 +17704,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>476</v>
       </c>
@@ -17730,7 +17745,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>484</v>
       </c>
@@ -17771,7 +17786,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>490</v>
       </c>
@@ -17815,7 +17830,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>498</v>
       </c>
@@ -17850,7 +17865,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>504</v>
       </c>
@@ -17882,7 +17897,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>510</v>
       </c>
@@ -17917,7 +17932,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>514</v>
       </c>
@@ -17949,7 +17964,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>517</v>
       </c>
@@ -17972,7 +17987,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>520</v>
       </c>
@@ -17995,7 +18010,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>523</v>
       </c>
@@ -18015,7 +18030,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
         <v>526</v>
       </c>
@@ -18035,7 +18050,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
         <v>529</v>
       </c>
@@ -18058,7 +18073,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
         <v>532</v>
       </c>
@@ -18081,7 +18096,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
         <v>535</v>
       </c>
@@ -18101,7 +18116,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
         <v>539</v>
       </c>
@@ -18121,7 +18136,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
         <v>543</v>
       </c>
@@ -18135,7 +18150,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
         <v>547</v>
       </c>
@@ -18158,7 +18173,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
         <v>552</v>
       </c>
@@ -18178,7 +18193,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
         <v>557</v>
       </c>
@@ -18195,7 +18210,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
         <v>562</v>
       </c>
@@ -18230,7 +18245,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
         <v>568</v>
       </c>
@@ -18259,7 +18274,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
         <v>573</v>
       </c>
@@ -18288,7 +18303,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
         <v>578</v>
       </c>
@@ -18314,7 +18329,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
         <v>581</v>
       </c>
@@ -18328,7 +18343,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
         <v>585</v>
       </c>
@@ -18342,7 +18357,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1" t="s">
         <v>590</v>
       </c>
@@ -18368,7 +18383,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
         <v>594</v>
       </c>
@@ -18394,7 +18409,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
         <v>599</v>
       </c>
@@ -18433,36 +18448,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.41796875" customWidth="1"/>
+    <col min="5" max="5" width="11.41796875" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>697</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>701</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="11" t="s">
         <v>614</v>
       </c>
@@ -18473,13 +18488,13 @@
         <v>663</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>702</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>663</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>681</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>681</v>
+        <v>702</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>681</v>
@@ -18493,8 +18508,14 @@
       <c r="J2" s="7" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="K2" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="10" t="s">
         <v>688</v>
       </c>
@@ -18503,28 +18524,34 @@
         <v>685</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>699</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>686</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>689</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>692</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>695</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>696</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
         <v>657</v>
       </c>
@@ -18534,14 +18561,14 @@
       <c r="C4" s="11" t="s">
         <v>664</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>665</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>682</v>
+        <v>665</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>682</v>
+        <v>664</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>682</v>
@@ -18555,8 +18582,14 @@
       <c r="J4" s="11" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="11" t="s">
+        <v>682</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7" t="s">
         <v>658</v>
       </c>
@@ -18566,23 +18599,29 @@
       <c r="C5" s="11" t="s">
         <v>666</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="12" t="s">
+        <v>667</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>666</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>683</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="H5" s="7" t="s">
         <v>683</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="11" t="s">
         <v>659</v>
       </c>
@@ -18592,23 +18631,29 @@
       <c r="C6" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="12" t="s">
+        <v>664</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>690</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="L6" s="7" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="7" t="s">
         <v>661</v>
       </c>
@@ -18618,55 +18663,72 @@
       <c r="C7" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="12" t="s">
+        <v>666</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>691</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>684</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="L7" s="7" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>698</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+    <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="15" t="s">
+        <v>697</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="13" t="s">
+        <v>703</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="14" t="s">
         <v>680</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="8" t="s">
         <v>618</v>
       </c>
@@ -18686,7 +18748,7 @@
         <v>672</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>673</v>
@@ -18698,7 +18760,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>0</v>
       </c>
@@ -18730,7 +18792,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>1</v>
       </c>
@@ -18762,7 +18824,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>2</v>
       </c>
@@ -18794,7 +18856,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>3</v>
       </c>
@@ -18826,7 +18888,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>4</v>
       </c>
@@ -18859,10 +18921,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A16:J16"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="B9:D11"/>
+    <mergeCell ref="E9:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>